<commit_message>
Před vytvořením Směrného plánu 3
</commit_message>
<xml_diff>
--- a/414_003_T02_RP.xlsx
+++ b/414_003_T02_RP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vse-my.sharepoint.com/personal/posm04_vse_cz/Documents/ZS2020/Řízení_projektů/MS Project REPO/MS-Project-4IT414/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{60181E14-34DB-4A46-A511-8E0CD0EC61F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="6_{60181E14-34DB-4A46-A511-8E0CD0EC61F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C93B049-3C64-4571-B23E-5472EB87BE4F}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1234,10 +1234,10 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K36" sqref="K4:K36"/>
+      <selection pane="bottomRight" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="H4" s="23">
         <f ca="1">LN(_xlfn.LOGNORM.INV(RAND(),F4,G4))</f>
-        <v>76.509723715797449</v>
+        <v>84.239183971609293</v>
       </c>
       <c r="I4" s="35">
         <f ca="1">ROUND(IF(G4=0,F4,IF(H4&lt;F4,F4,H4)),$M$3)</f>
@@ -1391,11 +1391,11 @@
       </c>
       <c r="H5" s="23">
         <f t="shared" ref="H5:H58" ca="1" si="3">LN(_xlfn.LOGNORM.INV(RAND(),F5,G5))</f>
-        <v>3.7426628550347862</v>
+        <v>3.1566675237904427</v>
       </c>
       <c r="I5" s="35">
         <f t="shared" ref="I5:I58" ca="1" si="4">ROUND(IF(G5=0,F5,IF(H5&lt;F5,F5,H5)),$M$3)</f>
-        <v>3.74</v>
+        <v>3.16</v>
       </c>
       <c r="J5" s="28"/>
       <c r="K5" s="39">
@@ -1428,11 +1428,11 @@
       </c>
       <c r="H6" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2936499891988773</v>
+        <v>3.9170443868729068</v>
       </c>
       <c r="I6" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.29</v>
+        <v>3.92</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="39">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="H7" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.4077875160347038</v>
+        <v>4.2916266690622997</v>
       </c>
       <c r="I7" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.41</v>
+        <v>4.29</v>
       </c>
       <c r="J7" s="28"/>
       <c r="K7" s="39">
@@ -1502,11 +1502,11 @@
       </c>
       <c r="H8" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.2184012771051833</v>
+        <v>5.8788280983553323</v>
       </c>
       <c r="I8" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.22</v>
+        <v>5.88</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="39">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="H9" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5273301147350247</v>
+        <v>2.2951243331548836</v>
       </c>
       <c r="I9" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1576,11 +1576,11 @@
       </c>
       <c r="H10" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>11.586524418950049</v>
+        <v>9.0872972146823976</v>
       </c>
       <c r="I10" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>11.59</v>
+        <v>10</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="39">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="H11" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5731996211992989</v>
+        <v>5.1641245646086738</v>
       </c>
       <c r="I11" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4.83</v>
+        <v>5.16</v>
       </c>
       <c r="J11" s="28"/>
       <c r="K11" s="39">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="H12" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8010068087242308</v>
+        <v>1.1287201388002082</v>
       </c>
       <c r="I12" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1687,11 +1687,11 @@
       </c>
       <c r="H13" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.1361986515784093</v>
+        <v>4.5630170193259518</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4.1399999999999997</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="J13" s="28"/>
       <c r="K13" s="39">
@@ -1724,11 +1724,11 @@
       </c>
       <c r="H14" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.7277181261835035</v>
+        <v>3.4088333904978159</v>
       </c>
       <c r="I14" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.41</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="39">
@@ -1761,11 +1761,11 @@
       </c>
       <c r="H15" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.6612180290147442</v>
+        <v>9.7644984624012476</v>
       </c>
       <c r="I15" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>8.17</v>
+        <v>9.76</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="39">
@@ -1798,11 +1798,11 @@
       </c>
       <c r="H16" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.8158047537448923</v>
+        <v>6.2670875447892067</v>
       </c>
       <c r="I16" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>7.82</v>
+        <v>7</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="39">
@@ -1835,11 +1835,11 @@
       </c>
       <c r="H17" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>9.4556784513624894</v>
+        <v>10.733755683029159</v>
       </c>
       <c r="I17" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>10.73</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="39">
@@ -1872,11 +1872,11 @@
       </c>
       <c r="H18" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.9837069238643923</v>
+        <v>4.3709584744614656</v>
       </c>
       <c r="I18" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>4.37</v>
       </c>
       <c r="J18" s="28"/>
       <c r="K18" s="39">
@@ -1909,11 +1909,11 @@
       </c>
       <c r="H19" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>6.9138964933889655</v>
+        <v>8.7777237123479033</v>
       </c>
       <c r="I19" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>8.17</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="39">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="H20" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1723382113804419</v>
+        <v>10.830519735509213</v>
       </c>
       <c r="I20" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>10.83</v>
       </c>
       <c r="J20" s="28"/>
       <c r="K20" s="39">
@@ -1983,11 +1983,11 @@
       </c>
       <c r="H21" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.9198494859400559</v>
+        <v>4.5289747956467625</v>
       </c>
       <c r="I21" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>4.53</v>
       </c>
       <c r="J21" s="28"/>
       <c r="K21" s="39">
@@ -2020,11 +2020,11 @@
       </c>
       <c r="H22" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.759144529114514</v>
+        <v>4.3485911011065328</v>
       </c>
       <c r="I22" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4.76</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="J22" s="28"/>
       <c r="K22" s="39">
@@ -2060,11 +2060,11 @@
       </c>
       <c r="H23" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>34.384232500215454</v>
+        <v>26.213872717644772</v>
       </c>
       <c r="I23" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>34.380000000000003</v>
+        <v>26.83</v>
       </c>
       <c r="J23" s="28"/>
       <c r="K23" s="39">
@@ -2097,11 +2097,11 @@
       </c>
       <c r="H24" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.2496609401603509</v>
+        <v>4.1572132334746925</v>
       </c>
       <c r="I24" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4.25</v>
+        <v>4.16</v>
       </c>
       <c r="J24" s="28"/>
       <c r="K24" s="39">
@@ -2134,11 +2134,11 @@
       </c>
       <c r="H25" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1455544616110793</v>
+        <v>2.5042468227716217</v>
       </c>
       <c r="I25" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.15</v>
+        <v>2.5</v>
       </c>
       <c r="J25" s="28"/>
       <c r="K25" s="39">
@@ -2171,11 +2171,11 @@
       </c>
       <c r="H26" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.0091692505926155</v>
+        <v>1.82150377677185</v>
       </c>
       <c r="I26" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.01</v>
+        <v>2.17</v>
       </c>
       <c r="J26" s="28"/>
       <c r="K26" s="39">
@@ -2208,11 +2208,11 @@
       </c>
       <c r="H27" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9953345698006513</v>
+        <v>0.64527566641333811</v>
       </c>
       <c r="I27" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2.17</v>
       </c>
       <c r="J27" s="28"/>
       <c r="K27" s="39">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="H28" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.0577378395235004</v>
+        <v>1.3529710269494535</v>
       </c>
       <c r="I28" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.06</v>
+        <v>2</v>
       </c>
       <c r="J28" s="28"/>
       <c r="K28" s="39">
@@ -2282,11 +2282,11 @@
       </c>
       <c r="H29" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.97255792263095</v>
+        <v>4.2307779780860413</v>
       </c>
       <c r="I29" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="J29" s="28"/>
       <c r="K29" s="39">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="H30" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.79820094511172535</v>
+        <v>1.8233245507239051</v>
       </c>
       <c r="I30" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2356,11 +2356,11 @@
       </c>
       <c r="H31" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9510564804768074</v>
+        <v>2.442384155622781</v>
       </c>
       <c r="I31" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.17</v>
+        <v>2.44</v>
       </c>
       <c r="J31" s="28"/>
       <c r="K31" s="39">
@@ -2393,11 +2393,11 @@
       </c>
       <c r="H32" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3535974985127917</v>
+        <v>2.5524775799582526</v>
       </c>
       <c r="I32" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.35</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="J32" s="28"/>
       <c r="K32" s="39">
@@ -2430,11 +2430,11 @@
       </c>
       <c r="H33" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5237868066532985</v>
+        <v>2.4816449497950734</v>
       </c>
       <c r="I33" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.48</v>
       </c>
       <c r="J33" s="28"/>
       <c r="K33" s="39">
@@ -2467,11 +2467,11 @@
       </c>
       <c r="H34" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7607883693930548</v>
+        <v>2.1580872818792627</v>
       </c>
       <c r="I34" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.16</v>
       </c>
       <c r="J34" s="28"/>
       <c r="K34" s="39">
@@ -2487,31 +2487,31 @@
       </c>
       <c r="C35" s="42">
         <f>SUM(C36:C51)</f>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D35" s="42">
         <f t="shared" ref="D35:E35" si="6">SUM(D36:D51)</f>
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E35" s="42">
         <f t="shared" si="6"/>
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="1"/>
-        <v>153.33333333333334</v>
+        <v>156.5</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="2"/>
-        <v>39.5</v>
+        <v>40.75</v>
       </c>
       <c r="H35" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>214.22082871643877</v>
+        <v>158.85123765590501</v>
       </c>
       <c r="I35" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>214.22</v>
+        <v>158.85</v>
       </c>
       <c r="J35" s="28"/>
       <c r="K35" s="39">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="H36" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.2645977185457911</v>
+        <v>2.801077286019753</v>
       </c>
       <c r="I36" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.26</v>
+        <v>5.17</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="39">
@@ -2581,11 +2581,11 @@
       </c>
       <c r="H37" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5322520377265167</v>
+        <v>6.711075711581171</v>
       </c>
       <c r="I37" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>6.17</v>
+        <v>6.71</v>
       </c>
       <c r="J37" s="28"/>
       <c r="K37" s="39">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="H38" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>19.90928904715426</v>
+        <v>34.867968960379024</v>
       </c>
       <c r="I38" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2655,11 +2655,11 @@
       </c>
       <c r="H39" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5987209295923837</v>
+        <v>4.5757026257880273</v>
       </c>
       <c r="I39" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.6</v>
+        <v>5.17</v>
       </c>
       <c r="J39" s="28"/>
       <c r="K39" s="39">
@@ -2692,11 +2692,11 @@
       </c>
       <c r="H40" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>9.883000807925038</v>
+        <v>4.9630500363930405</v>
       </c>
       <c r="I40" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>9.8800000000000008</v>
+        <v>9.5</v>
       </c>
       <c r="J40" s="28"/>
       <c r="K40" s="39">
@@ -2729,11 +2729,11 @@
       </c>
       <c r="H41" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.6344589709969837</v>
+        <v>6.8261556527198</v>
       </c>
       <c r="I41" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>6.83</v>
       </c>
       <c r="J41" s="28"/>
       <c r="K41" s="39">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="H42" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6193435635461153</v>
+        <v>1.9826662949432265</v>
       </c>
       <c r="I42" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="H43" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.8190106570731173</v>
+        <v>5.1093192739760536</v>
       </c>
       <c r="I43" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2840,11 +2840,11 @@
       </c>
       <c r="H44" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>16.009796493671097</v>
+        <v>22.30017931690475</v>
       </c>
       <c r="I44" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>20</v>
+        <v>22.3</v>
       </c>
       <c r="J44" s="28"/>
       <c r="K44" s="39">
@@ -2877,11 +2877,11 @@
       </c>
       <c r="H45" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1780469388101587</v>
+        <v>15.116261871328597</v>
       </c>
       <c r="I45" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>15.12</v>
       </c>
       <c r="J45" s="28"/>
       <c r="K45" s="39">
@@ -2914,11 +2914,11 @@
       </c>
       <c r="H46" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>22.795919520790278</v>
+        <v>13.087092649920134</v>
       </c>
       <c r="I46" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>22.8</v>
+        <v>20</v>
       </c>
       <c r="J46" s="28"/>
       <c r="K46" s="39">
@@ -2951,11 +2951,11 @@
       </c>
       <c r="H47" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.0034898102589924</v>
+        <v>6.3519286079476283</v>
       </c>
       <c r="I47" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.17</v>
+        <v>6.35</v>
       </c>
       <c r="J47" s="28"/>
       <c r="K47" s="39">
@@ -2970,33 +2970,33 @@
         <v>57</v>
       </c>
       <c r="C48" s="43">
+        <v>2</v>
+      </c>
+      <c r="D48" s="43">
+        <v>4</v>
+      </c>
+      <c r="E48" s="43">
+        <v>6</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G48" s="4">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D48" s="43">
-        <v>2</v>
-      </c>
-      <c r="E48" s="43">
-        <v>3</v>
-      </c>
-      <c r="F48" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G48" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
       <c r="H48" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4911955989377619</v>
+        <v>4.2906740618507966</v>
       </c>
       <c r="I48" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4.29</v>
       </c>
       <c r="J48" s="28"/>
       <c r="K48" s="39">
-        <v>2</v>
+        <v>4.09</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -3010,30 +3010,30 @@
         <v>1</v>
       </c>
       <c r="D49" s="43">
+        <v>2</v>
+      </c>
+      <c r="E49" s="43">
+        <v>5</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="G49" s="4">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E49" s="43">
-        <v>2</v>
-      </c>
-      <c r="F49" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="G49" s="4">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
       <c r="H49" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2256743754285364</v>
+        <v>2.5087327862176734</v>
       </c>
       <c r="I49" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>1.23</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="J49" s="28"/>
       <c r="K49" s="39">
-        <v>1.28</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -3062,11 +3062,11 @@
       </c>
       <c r="H50" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>12.745222303711877</v>
+        <v>5.5913579072411075</v>
       </c>
       <c r="I50" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>12.75</v>
+        <v>10</v>
       </c>
       <c r="J50" s="28"/>
       <c r="K50" s="39">
@@ -3099,11 +3099,11 @@
       </c>
       <c r="H51" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>14.149524913779789</v>
+        <v>10.44090036103376</v>
       </c>
       <c r="I51" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>14.15</v>
+        <v>10.44</v>
       </c>
       <c r="J51" s="28"/>
       <c r="K51" s="39">
@@ -3139,7 +3139,7 @@
       </c>
       <c r="H52" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>28.689093743737278</v>
+        <v>26.218396931040637</v>
       </c>
       <c r="I52" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3176,11 +3176,11 @@
       </c>
       <c r="H53" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5920160706323694</v>
+        <v>4.4048685275013018</v>
       </c>
       <c r="I53" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.17</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J53" s="28"/>
       <c r="K53" s="39">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="H54" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1216815618064473</v>
+        <v>0.70226674241510312</v>
       </c>
       <c r="I54" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="H55" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7926198376510052</v>
+        <v>1.4682184350456988</v>
       </c>
       <c r="I55" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3287,11 +3287,11 @@
       </c>
       <c r="H56" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>14.615164786231574</v>
+        <v>16.188248937700671</v>
       </c>
       <c r="I56" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>14.83</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="J56" s="28"/>
       <c r="K56" s="39">
@@ -3324,11 +3324,11 @@
       </c>
       <c r="H57" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>6.6798026046617647</v>
+        <v>6.5181690344046901</v>
       </c>
       <c r="I57" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>6.68</v>
+        <v>6.52</v>
       </c>
       <c r="J57" s="28"/>
       <c r="K57" s="39">
@@ -3361,11 +3361,11 @@
       </c>
       <c r="H58" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.400120286267438</v>
+        <v>3.5869992630716472</v>
       </c>
       <c r="I58" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.4</v>
+        <v>3.59</v>
       </c>
       <c r="J58" s="28"/>
       <c r="K58" s="39">

</xml_diff>